<commit_message>
Updated the existed POM Framework for ADDA and IPMS
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginTest" sheetId="2" r:id="rId1"/>
+    <sheet name="loginADDA" sheetId="2" r:id="rId1"/>
+    <sheet name="loginIPMST" sheetId="4" r:id="rId2"/>
+    <sheet name="invalidLoginTest" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>fullName</t>
   </si>
@@ -36,6 +38,9 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -437,7 +442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -462,10 +469,79 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1CD5F2-3D77-4285-A847-3C325985CED7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3924DB8F-48F0-40AD-ACFD-444AC562CF68}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Admin login with valid username and password
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,12 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginADDA" sheetId="2" r:id="rId1"/>
-    <sheet name="loginIPMST" sheetId="4" r:id="rId2"/>
-    <sheet name="invalidLoginTest" sheetId="3" r:id="rId3"/>
+    <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>fullName</t>
   </si>
@@ -34,13 +32,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>archadda_admin</t>
+    <t>admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>userType</t>
   </si>
 </sst>
 </file>
@@ -439,106 +434,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1CD5F2-3D77-4285-A847-3C325985CED7}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1CD5F2-3D77-4285-A847-3C325985CED7}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3924DB8F-48F0-40AD-ACFD-444AC562CF68}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented for checking SharePoint submenu title in dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
+    <sheet name="checkSharePointSubmenuTitle" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>fullName</t>
   </si>
@@ -36,6 +37,12 @@
   </si>
   <si>
     <t>userType</t>
+  </si>
+  <si>
+    <t>submenuTitleName</t>
+  </si>
+  <si>
+    <t>SharePoint</t>
   </si>
 </sst>
 </file>
@@ -92,8 +99,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -437,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1CD5F2-3D77-4285-A847-3C325985CED7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -469,4 +482,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAB93B1-3D9F-4817-84B0-1FCD0FD56B02}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Successfully checked the horizontal groups in Horizontal Groups Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
     <sheet name="checkSharePointSubmenuTitle" sheetId="5" r:id="rId2"/>
+    <sheet name="dashboardHorizontalGroups" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>fullName</t>
   </si>
@@ -43,13 +44,49 @@
   </si>
   <si>
     <t>SharePoint</t>
+  </si>
+  <si>
+    <t>submenuTitle</t>
+  </si>
+  <si>
+    <t>Horizontal Groups Dashboard</t>
+  </si>
+  <si>
+    <t>innerSubmenuTitle</t>
+  </si>
+  <si>
+    <t>HORIZONTAL GROUPS</t>
+  </si>
+  <si>
+    <t>/resources/images/group-images/business.png</t>
+  </si>
+  <si>
+    <t>groupNameLearningAndDiffusionGroupPath</t>
+  </si>
+  <si>
+    <t>groupNameBusinessPath</t>
+  </si>
+  <si>
+    <t>groupNamePolicyAndProgramsPath</t>
+  </si>
+  <si>
+    <t>groupNameResearchPath</t>
+  </si>
+  <si>
+    <t>/resources/images/group-images/Research.png</t>
+  </si>
+  <si>
+    <t>/resources/images/group-images/Learning%20and%20diffusion%20Group.png</t>
+  </si>
+  <si>
+    <t>/resources/images/group-images/policy%20and%20programs.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +113,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,13 +142,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -488,9 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAB93B1-3D9F-4817-84B0-1FCD0FD56B02}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -510,4 +557,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48050845-CDAD-44F3-9B71-439EE59EB254}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="33.375" customWidth="1"/>
+    <col min="2" max="2" width="21.25" customWidth="1"/>
+    <col min="3" max="3" width="43.5" customWidth="1"/>
+    <col min="4" max="4" width="74.25" customWidth="1"/>
+    <col min="5" max="5" width="36.875" customWidth="1"/>
+    <col min="6" max="6" width="25.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31.5">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the Add Meeting, View Meeting and Update Meeting in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
     <sheet name="checkSharePointSubmenuTitle" sheetId="5" r:id="rId2"/>
     <sheet name="dashboardHorizontalGroups" sheetId="6" r:id="rId3"/>
+    <sheet name="meetingsManagement" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>fullName</t>
   </si>
@@ -80,6 +81,72 @@
   </si>
   <si>
     <t>/resources/images/group-images/policy%20and%20programs.png</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>organizer</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>confCall</t>
+  </si>
+  <si>
+    <t>facilitator</t>
+  </si>
+  <si>
+    <t>verticalGroup</t>
+  </si>
+  <si>
+    <t>editTitleHeading</t>
+  </si>
+  <si>
+    <t>updatedMeetingSuccessMessage</t>
+  </si>
+  <si>
+    <t>Meeting Updated Successfully.</t>
+  </si>
+  <si>
+    <t>20/12/2017</t>
+  </si>
+  <si>
+    <t>1AM</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Million Hearts (MH)</t>
+  </si>
+  <si>
+    <t>updateTitle</t>
+  </si>
+  <si>
+    <t>EDIT MEETING</t>
+  </si>
+  <si>
+    <t>TestignTitle11</t>
+  </si>
+  <si>
+    <t>TestingTitle22</t>
   </si>
 </sst>
 </file>
@@ -563,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48050845-CDAD-44F3-9B71-439EE59EB254}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -621,4 +688,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CEAE1B-ED93-444F-81B3-7F03F261FF24}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="7" max="7" width="11.25" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="10" max="10" width="21.625" customWidth="1"/>
+    <col min="11" max="11" width="25.375" customWidth="1"/>
+    <col min="12" max="12" width="15.125" customWidth="1"/>
+    <col min="13" max="13" width="35.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>12345678</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the Add Task, Upload Tasks and View Tasks in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
     <sheet name="checkSharePointSubmenuTitle" sheetId="5" r:id="rId2"/>
     <sheet name="dashboardHorizontalGroups" sheetId="6" r:id="rId3"/>
     <sheet name="meetingsManagement" sheetId="7" r:id="rId4"/>
+    <sheet name="taskManagement" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>fullName</t>
   </si>
@@ -147,6 +148,24 @@
   </si>
   <si>
     <t>TestingTitle22</t>
+  </si>
+  <si>
+    <t>addTask</t>
+  </si>
+  <si>
+    <t>uploadTasks</t>
+  </si>
+  <si>
+    <t>viewTasks</t>
+  </si>
+  <si>
+    <t>Add Task</t>
+  </si>
+  <si>
+    <t>Upload Tasks</t>
+  </si>
+  <si>
+    <t>View Tasks</t>
   </si>
 </sst>
 </file>
@@ -694,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CEAE1B-ED93-444F-81B3-7F03F261FF24}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -795,4 +814,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA15649B-3EDF-4EB8-85CD-177F388AB2BC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the EVM Upload, Financial Report and EVM Metrics of Financial Management in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="dashboardHorizontalGroups" sheetId="6" r:id="rId3"/>
     <sheet name="meetingsManagement" sheetId="7" r:id="rId4"/>
     <sheet name="taskManagement" sheetId="8" r:id="rId5"/>
+    <sheet name="finacialManagement" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>fullName</t>
   </si>
@@ -166,6 +167,21 @@
   </si>
   <si>
     <t>View Tasks</t>
+  </si>
+  <si>
+    <t>evmUploadTitle</t>
+  </si>
+  <si>
+    <t>EVM Upload</t>
+  </si>
+  <si>
+    <t>finacialReportTitle</t>
+  </si>
+  <si>
+    <t>Financial Report</t>
+  </si>
+  <si>
+    <t>EVM Metrics</t>
   </si>
 </sst>
 </file>
@@ -820,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA15649B-3EDF-4EB8-85CD-177F388AB2BC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -856,4 +872,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6E555D-38FE-4676-9D69-C0BA411A2B0D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the Add Issue, Upload Issues, View Issues of Issue Management in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="meetingsManagement" sheetId="7" r:id="rId4"/>
     <sheet name="taskManagement" sheetId="8" r:id="rId5"/>
     <sheet name="finacialManagement" sheetId="9" r:id="rId6"/>
+    <sheet name="issueManagement" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>fullName</t>
   </si>
@@ -182,6 +183,30 @@
   </si>
   <si>
     <t>EVM Metrics</t>
+  </si>
+  <si>
+    <t>addIssueTitle</t>
+  </si>
+  <si>
+    <t>uploadIssuesTitle</t>
+  </si>
+  <si>
+    <t>searchIssuesTitle</t>
+  </si>
+  <si>
+    <t>viewIssueTitle</t>
+  </si>
+  <si>
+    <t>Add Issue</t>
+  </si>
+  <si>
+    <t>Upload Issues</t>
+  </si>
+  <si>
+    <t>Search Issues(JIRA)</t>
+  </si>
+  <si>
+    <t>View Issues</t>
   </si>
 </sst>
 </file>
@@ -244,7 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -258,6 +283,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -878,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6E555D-38FE-4676-9D69-C0BA411A2B0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -914,4 +940,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1AB562-B801-4630-A448-89C78D890120}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the Add Risk, Upload Risks and View Risks of Risk Management in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="taskManagement" sheetId="8" r:id="rId5"/>
     <sheet name="finacialManagement" sheetId="9" r:id="rId6"/>
     <sheet name="issueManagement" sheetId="10" r:id="rId7"/>
+    <sheet name="riskManagement" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>fullName</t>
   </si>
@@ -207,6 +208,24 @@
   </si>
   <si>
     <t>View Issues</t>
+  </si>
+  <si>
+    <t>addRisk</t>
+  </si>
+  <si>
+    <t>uploadRisks</t>
+  </si>
+  <si>
+    <t>viewRisks</t>
+  </si>
+  <si>
+    <t>Add Risk</t>
+  </si>
+  <si>
+    <t>Upload Risks</t>
+  </si>
+  <si>
+    <t>View Risks</t>
   </si>
 </sst>
 </file>
@@ -946,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1AB562-B801-4630-A448-89C78D890120}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -990,4 +1009,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DEFB8D-146B-4F84-8DF1-A8F9312DB14B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the Upload Lessons Learned, View Lessons Learned and View Action Items of Add Project in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="finacialManagement" sheetId="9" r:id="rId6"/>
     <sheet name="issueManagement" sheetId="10" r:id="rId7"/>
     <sheet name="riskManagement" sheetId="11" r:id="rId8"/>
+    <sheet name="addProject" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>fullName</t>
   </si>
@@ -226,6 +227,30 @@
   </si>
   <si>
     <t>View Risks</t>
+  </si>
+  <si>
+    <t>uploadLessonsLearnedTitle</t>
+  </si>
+  <si>
+    <t>viewLessonsLearnedTitle</t>
+  </si>
+  <si>
+    <t>uploadActionItemsTitle</t>
+  </si>
+  <si>
+    <t>viewActionItemsTitle</t>
+  </si>
+  <si>
+    <t>Upload Lessons Learned</t>
+  </si>
+  <si>
+    <t>View Lessons Learned</t>
+  </si>
+  <si>
+    <t>Upload Action Items</t>
+  </si>
+  <si>
+    <t>View Action items</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DEFB8D-146B-4F84-8DF1-A8F9312DB14B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1051,4 +1076,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FDC8D1-43EC-4F5C-B880-78E99EA79315}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="26.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="3" max="4" width="26.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tested Successfully for MS Project Integration button  in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="issueManagement" sheetId="10" r:id="rId7"/>
     <sheet name="riskManagement" sheetId="11" r:id="rId8"/>
     <sheet name="addProject" sheetId="12" r:id="rId9"/>
+    <sheet name="checkMSProjectIntegration" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>fullName</t>
   </si>
@@ -251,6 +252,12 @@
   </si>
   <si>
     <t>View Action items</t>
+  </si>
+  <si>
+    <t>msProjectIntegrationTitle</t>
+  </si>
+  <si>
+    <t>MS Project Integration</t>
   </si>
 </sst>
 </file>
@@ -705,6 +712,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF12738-C44D-4045-9484-A9D464A9498F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DAB93B1-3D9F-4817-84B0-1FCD0FD56B02}">
   <dimension ref="A1:A2"/>
@@ -1082,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FDC8D1-43EC-4F5C-B880-78E99EA79315}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tested Successfully for  Artifacts Manager in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="riskManagement" sheetId="11" r:id="rId8"/>
     <sheet name="addProject" sheetId="12" r:id="rId9"/>
     <sheet name="checkMSProjectIntegration" sheetId="13" r:id="rId10"/>
+    <sheet name="checkArtifactsManager" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>fullName</t>
   </si>
@@ -258,6 +259,12 @@
   </si>
   <si>
     <t>MS Project Integration</t>
+  </si>
+  <si>
+    <t>artifactsManagerTitle</t>
+  </si>
+  <si>
+    <t>Artifacts Manager</t>
   </si>
 </sst>
 </file>
@@ -716,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF12738-C44D-4045-9484-A9D464A9498F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -733,6 +740,34 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93E22A3-410A-40E9-BE7D-81E6160AAEBF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested successfully the View Projects in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test_data.xlsx
+++ b/src/test/resources/excel/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="2625" tabRatio="500" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginIPMS" sheetId="4" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="addProject" sheetId="12" r:id="rId9"/>
     <sheet name="checkMSProjectIntegration" sheetId="13" r:id="rId10"/>
     <sheet name="checkArtifactsManager" sheetId="14" r:id="rId11"/>
+    <sheet name="checkViewProjects" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>fullName</t>
   </si>
@@ -265,6 +266,12 @@
   </si>
   <si>
     <t>Artifacts Manager</t>
+  </si>
+  <si>
+    <t>viewProjectsTitle</t>
+  </si>
+  <si>
+    <t>View Projects</t>
   </si>
 </sst>
 </file>
@@ -751,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93E22A3-410A-40E9-BE7D-81E6160AAEBF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -768,6 +775,34 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4C4584-A1B9-4022-A0DC-9BC15657F0BF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="28.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>